<commit_message>
added more entry points
</commit_message>
<xml_diff>
--- a/stats_proj_data.xlsx
+++ b/stats_proj_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louiscerda/Desktop/CPSC/stats/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF03A9CC-C500-7D49-8B03-CB91D4768362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB24D16-DFC2-7E46-B2E6-C9927EA8DE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="760" windowWidth="28040" windowHeight="17240" xr2:uid="{605DF7E2-A4BA-2745-BAA5-67F2613E5E2E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="11">
   <si>
     <t>Age</t>
   </si>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C5092C-9250-1045-95B3-79E16214F4D5}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="159" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1023,11 +1023,89 @@
         <v>6</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>16</v>
+      </c>
+      <c r="C41">
+        <v>118</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>19</v>
+      </c>
+      <c r="C42">
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43">
+        <v>24</v>
+      </c>
+      <c r="C43">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44">
+        <v>19</v>
+      </c>
+      <c r="C44">
+        <v>62</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45">
+        <v>19</v>
+      </c>
+      <c r="C45">
+        <v>112</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
+      <c r="A46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>19</v>
+      </c>
+      <c r="C46">
+        <v>107</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>

</xml_diff>

<commit_message>
modified data and added graphs/correlations
</commit_message>
<xml_diff>
--- a/stats_proj_data.xlsx
+++ b/stats_proj_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louiscerda/Desktop/CPSC/stats/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB24D16-DFC2-7E46-B2E6-C9927EA8DE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDA0DC6-1F16-894A-8CEB-16643CC59530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="760" windowWidth="28040" windowHeight="17240" xr2:uid="{605DF7E2-A4BA-2745-BAA5-67F2613E5E2E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="10">
   <si>
     <t>Age</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>seen</t>
-  </si>
-  <si>
-    <t>Told</t>
   </si>
   <si>
     <t xml:space="preserve">Female </t>
@@ -451,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C5092C-9250-1045-95B3-79E16214F4D5}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="159" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="159" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,10 +468,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -488,7 +485,7 @@
         <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -516,7 +513,7 @@
         <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -628,7 +625,7 @@
         <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -698,7 +695,7 @@
         <v>180</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -726,7 +723,7 @@
         <v>150</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -754,12 +751,12 @@
         <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22">
         <v>31</v>
@@ -1108,18 +1105,76 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
+      <c r="A47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>48</v>
+      </c>
+      <c r="C47">
+        <v>66</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>45</v>
+      </c>
+      <c r="C48">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>20</v>
+      </c>
+      <c r="C49">
+        <v>83</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>19</v>
+      </c>
+      <c r="C50">
+        <v>132</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>21</v>
+      </c>
+      <c r="C51">
+        <v>89</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
     </row>
   </sheetData>

</xml_diff>